<commit_message>
applied to a few more places make sure I studygit push origin main!
</commit_message>
<xml_diff>
--- a/Employment/Employment Status.xlsx
+++ b/Employment/Employment Status.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gsh04\Desktop\2024-Summer\Employment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803741AF-14D5-4822-8349-608D364B546E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C14739-AA5E-420C-A1CB-6A9A5C1B6F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="16305" xr2:uid="{E0539C40-DB60-4822-ABC1-759342AC433F}"/>
   </bookViews>
@@ -36,8 +36,90 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="7">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="3"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="4"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="6"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="7">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
+    <bk>
+      <rc t="1" v="3"/>
+    </bk>
+    <bk>
+      <rc t="1" v="4"/>
+    </bk>
+    <bk>
+      <rc t="1" v="5"/>
+    </bk>
+    <bk>
+      <rc t="1" v="6"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="69">
   <si>
     <t>Draper</t>
   </si>
@@ -184,6 +266,66 @@
   </si>
   <si>
     <t>https://jobs.lever.co/ltaresearch/3d95a27b-6183-42cc-a03c-23eea97461ad/apply?source=LinkedIn</t>
+  </si>
+  <si>
+    <t>Lockheed Martin</t>
+  </si>
+  <si>
+    <t>Guidance Navigation and Control Engineer (671543BR)</t>
+  </si>
+  <si>
+    <t>https://www.lockheedmartinjobs.com/job/huntsville/guidance-navigation-and-control-engineer/694/67985288720</t>
+  </si>
+  <si>
+    <t>Rnqhstjr12%</t>
+  </si>
+  <si>
+    <t>Guidance Navigation and Control Engineer (671541BR)</t>
+  </si>
+  <si>
+    <t>https://www.lockheedmartinjobs.com/job/huntsville/guidance-navigation-and-control-engineer/694/67985285744</t>
+  </si>
+  <si>
+    <t>Guidance Navigation and Control Engineer (671546BR)</t>
+  </si>
+  <si>
+    <t>https://www.lockheedmartinjobs.com/job/huntsville/guidance-navigation-and-control-engineer/694/67979830944</t>
+  </si>
+  <si>
+    <t>Boeing</t>
+  </si>
+  <si>
+    <t>Guidance Navigation and Control Engineer(00000435707)</t>
+  </si>
+  <si>
+    <t>https://jobs.boeing.com/job/saint-charles/guidance-navigation-and-control-engineer/185/68678951392</t>
+  </si>
+  <si>
+    <t>https://boards.greenhouse.io/relativity/jobs/7060327002?gh_jid=7060327002</t>
+  </si>
+  <si>
+    <t>Relativity Space</t>
+  </si>
+  <si>
+    <t>Software Simulation Engineer I</t>
+  </si>
+  <si>
+    <t>https://boards.greenhouse.io/spacex/jobs/7560266002?gh_jid=7560266002</t>
+  </si>
+  <si>
+    <t>GNC Engineer (Falcon)</t>
+  </si>
+  <si>
+    <t>https://boards.greenhouse.io/spacex/jobs/7550544002?gh_jid=7550544002</t>
+  </si>
+  <si>
+    <t>GNC Engineer (Starship) Hawthorn, CA</t>
+  </si>
+  <si>
+    <t>GNC Engineer (Starship) Starbase, TX</t>
+  </si>
+  <si>
+    <t>https://boards.greenhouse.io/spacex/jobs/7535388002?gh_jid=7535388002</t>
   </si>
 </sst>
 </file>
@@ -248,7 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -256,9 +398,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -275,6 +418,100 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="7">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>3</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>4</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>5</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>6</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
+  <rel r:id="rId4"/>
+  <rel r:id="rId5"/>
+  <rel r:id="rId6"/>
+  <rel r:id="rId7"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -574,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A248182B-F338-4D88-B5BE-882C43BCF2CB}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +825,7 @@
     <col min="4" max="4" width="55.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>26</v>
       </c>
@@ -602,119 +839,111 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5" s="2"/>
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="2"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="2"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="2"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="2"/>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="7"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="7"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9"/>
+      <c r="B13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="2"/>
+      <c r="D16" s="7"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="7"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C21" s="8">
@@ -724,8 +953,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="7" t="s">
+    <row r="22" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C22" s="8">
@@ -736,114 +965,174 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="D25" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="7"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="C30" s="2"/>
     </row>
     <row r="32" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
+      <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="B32"/>
+      <c r="C32" s="2"/>
+      <c r="D32"/>
+    </row>
+    <row r="34" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C34" s="8">
         <v>45467</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
       <c r="B36" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="2">
         <v>45467</v>
       </c>
       <c r="D36" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="8">
         <v>45467</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="6" t="s">
         <v>48</v>
       </c>
     </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" t="s">
+        <v>52</v>
+      </c>
+      <c r="G41" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F42" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="G42" t="e" vm="4">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D43" t="s">
+        <v>56</v>
+      </c>
+      <c r="F43" t="e" vm="5">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H43" t="e" vm="6">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H44" t="e" vm="7">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B47" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="2">
+        <v>45517</v>
+      </c>
+      <c r="D49" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D41" r:id="rId1" xr:uid="{C7F5CDCC-C64C-463C-926C-91C73641CC7B}"/>
+    <hyperlink ref="D42" r:id="rId2" xr:uid="{CE96B0B7-8DFE-4394-8492-12CA15B1D22A}"/>
+    <hyperlink ref="D47" r:id="rId3" xr:uid="{31996B9E-E760-4085-8FEA-64804E616A43}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>